<commit_message>
new run file for M1
</commit_message>
<xml_diff>
--- a/IO_ActMethods/RunControl_ActMethods.xlsx
+++ b/IO_ActMethods/RunControl_ActMethods.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="189">
   <si>
     <t>Sheet #</t>
   </si>
@@ -578,6 +578,24 @@
   </si>
   <si>
     <t>PUC_mc</t>
+  </si>
+  <si>
+    <t>EAN_Unif_ne</t>
+  </si>
+  <si>
+    <t>PUC_Unif_ne</t>
+  </si>
+  <si>
+    <t>EAN_Avg_ne</t>
+  </si>
+  <si>
+    <t>PUC_Avg_ne</t>
+  </si>
+  <si>
+    <t>EAN_mc_ne</t>
+  </si>
+  <si>
+    <t>PUC_mc_ne</t>
   </si>
 </sst>
 </file>
@@ -759,13 +777,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -774,10 +786,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1281,13 +1299,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ11"/>
+  <dimension ref="A1:AQ18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="U1" sqref="U1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,68 +1474,68 @@
       </c>
     </row>
     <row r="4" spans="1:43" s="8" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27" t="s">
+      <c r="E4" s="30"/>
+      <c r="F4" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28" t="s">
+      <c r="G4" s="31"/>
+      <c r="H4" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="29" t="s">
+      <c r="I4" s="26"/>
+      <c r="J4" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="28" t="s">
+      <c r="K4" s="27"/>
+      <c r="L4" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="29" t="s">
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="30" t="s">
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
       <c r="Y4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z4" s="25" t="s">
+      <c r="Z4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="31" t="s">
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="AD4" s="31"/>
-      <c r="AE4" s="31"/>
-      <c r="AF4" s="31"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
       <c r="AG4" s="17"/>
       <c r="AH4" s="24"/>
       <c r="AI4" s="22"/>
-      <c r="AJ4" s="30" t="s">
+      <c r="AJ4" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="AK4" s="30"/>
-      <c r="AL4" s="30"/>
+      <c r="AK4" s="25"/>
+      <c r="AL4" s="25"/>
       <c r="AM4" s="23" t="s">
         <v>70</v>
       </c>
@@ -2189,7 +2207,7 @@
         <v>181</v>
       </c>
       <c r="C10" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>109</v>
@@ -2320,7 +2338,7 @@
         <v>182</v>
       </c>
       <c r="C11" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>109</v>
@@ -2443,93 +2461,879 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I13" t="s">
+        <v>111</v>
+      </c>
+      <c r="J13" s="12">
+        <v>0</v>
+      </c>
+      <c r="K13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="N13">
+        <v>65</v>
+      </c>
+      <c r="O13">
+        <v>65</v>
+      </c>
+      <c r="P13" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q13">
+        <v>10</v>
+      </c>
+      <c r="R13">
+        <v>10</v>
+      </c>
+      <c r="S13" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T13" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U13" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V13" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="W13" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X13" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB13">
+        <v>20</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD13" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE13" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF13" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AG13" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK13" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AL13">
+        <v>200</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN13">
+        <v>5</v>
+      </c>
+      <c r="AO13">
+        <v>200</v>
+      </c>
+      <c r="AP13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I14" t="s">
+        <v>111</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>65</v>
+      </c>
+      <c r="O14">
+        <v>65</v>
+      </c>
+      <c r="P14" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>10</v>
+      </c>
+      <c r="S14" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T14" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U14" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V14" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="W14" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X14" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB14">
+        <v>20</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD14" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE14" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF14" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AG14" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK14" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AL14">
+        <v>200</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN14">
+        <v>5</v>
+      </c>
+      <c r="AO14">
+        <v>200</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" t="s">
+        <v>111</v>
+      </c>
+      <c r="J15" s="12">
+        <v>0</v>
+      </c>
+      <c r="K15" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>65</v>
+      </c>
+      <c r="O15">
+        <v>65</v>
+      </c>
+      <c r="P15" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q15">
+        <v>10</v>
+      </c>
+      <c r="R15">
+        <v>10</v>
+      </c>
+      <c r="S15" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T15" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U15" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V15" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="W15" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X15" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB15">
+        <v>20</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD15" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE15" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF15" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AG15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK15" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AL15">
+        <v>200</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN15">
+        <v>5</v>
+      </c>
+      <c r="AO15">
+        <v>200</v>
+      </c>
+      <c r="AP15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" t="s">
+        <v>111</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>65</v>
+      </c>
+      <c r="O16">
+        <v>65</v>
+      </c>
+      <c r="P16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q16">
+        <v>10</v>
+      </c>
+      <c r="R16">
+        <v>10</v>
+      </c>
+      <c r="S16" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U16" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V16" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="W16" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X16" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB16">
+        <v>20</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD16" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE16" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF16" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AG16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI16" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK16" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AL16">
+        <v>200</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN16">
+        <v>5</v>
+      </c>
+      <c r="AO16">
+        <v>200</v>
+      </c>
+      <c r="AP16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" t="s">
+        <v>111</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
+      <c r="K17" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <v>65</v>
+      </c>
+      <c r="O17">
+        <v>65</v>
+      </c>
+      <c r="P17" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q17">
+        <v>10</v>
+      </c>
+      <c r="R17">
+        <v>10</v>
+      </c>
+      <c r="S17" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T17" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U17" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V17" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="W17" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X17" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB17">
+        <v>20</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD17" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE17" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF17" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AG17" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI17" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK17" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AL17">
+        <v>200</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN17">
+        <v>5</v>
+      </c>
+      <c r="AO17">
+        <v>200</v>
+      </c>
+      <c r="AP17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" t="s">
+        <v>111</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>65</v>
+      </c>
+      <c r="O18">
+        <v>65</v>
+      </c>
+      <c r="P18" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="Q18">
+        <v>10</v>
+      </c>
+      <c r="R18">
+        <v>10</v>
+      </c>
+      <c r="S18" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="T18" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="U18" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="V18" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="W18" s="12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="X18" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB18">
+        <v>20</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD18" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="AE18" s="14">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AF18" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="AG18" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK18" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="AL18">
+        <v>200</v>
+      </c>
+      <c r="AM18" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN18">
+        <v>5</v>
+      </c>
+      <c r="AO18">
+        <v>200</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ18">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="AJ4:AL4"/>
     <mergeCell ref="L4:R4"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AC4:AF4"/>
     <mergeCell ref="V4:X4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <dataValidations count="20">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP11 AP13:AP18">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA6:AA11 AA13:AA18">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z6:Z11 Z13:Z18">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC6:AC11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC6:AC11 AC13:AC18">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K11 C6:C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K11 C6:C11 K13:K18 C13:C18">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="N6:N11 N13:N18">
       <formula1>55</formula1>
       <formula2>65</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P11 T6:T11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="P6:P11 T6:T11 P13:P18 T13:T18">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="Q6:R11 Q13:R18">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S11 W6:W11 U6:U11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="S6:S11 W6:W11 U6:U11 S13:S18 W13:W18 U13:U18">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AB6:AB11 AB13:AB18">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AD6:AE11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AD6:AE11 AD13:AE18">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AF6:AF11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AF6:AF11 AF13:AF18">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="X6:X11 X13:X18">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AN6:AN11">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AN6:AN11 AN13:AN18">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO11">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO11 AO13:AO18">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6:AQ11">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ6:AQ11 AQ13:AQ18">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V11"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AI11">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="V6:V11 V13:V18"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AI11 AG13:AI18">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ6:AJ11 AJ13:AJ18">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK6:AK11 AK13:AK18">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
@@ -2543,43 +3347,43 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$17:$A$18</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:D11</xm:sqref>
+          <xm:sqref>D6:D11 D13:D18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$21:$A$22</xm:f>
           </x14:formula1>
-          <xm:sqref>E6:E11</xm:sqref>
+          <xm:sqref>E6:E11 E13:E18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$29:$A$30</xm:f>
           </x14:formula1>
-          <xm:sqref>F6:F11</xm:sqref>
+          <xm:sqref>F6:F11 F13:F18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$25:$A$26</xm:f>
           </x14:formula1>
-          <xm:sqref>G6:G11</xm:sqref>
+          <xm:sqref>G6:G11 G13:G18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$37:$A$41</xm:f>
           </x14:formula1>
-          <xm:sqref>H6:H11</xm:sqref>
+          <xm:sqref>H6:H11 H13:H18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$44:$A$46</xm:f>
           </x14:formula1>
-          <xm:sqref>I6:I11</xm:sqref>
+          <xm:sqref>I6:I11 I13:I18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$7:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>Y6:Y11</xm:sqref>
+          <xm:sqref>Y6:Y11 Y13:Y18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>